<commit_message>
cambiando formato fecha en fotos cumpleaños
</commit_message>
<xml_diff>
--- a/cumpleaniosNyN.xlsx
+++ b/cumpleaniosNyN.xlsx
@@ -380,7 +380,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,7 +401,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -412,7 +412,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -423,7 +423,7 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -434,7 +434,7 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -445,7 +445,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -456,7 +456,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -478,7 +478,7 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>

</xml_diff>